<commit_message>
use of sikuli in to the test cases
</commit_message>
<xml_diff>
--- a/caphase3/src/test/java/com/softweb/cure/excels/LoginData.xlsx
+++ b/caphase3/src/test/java/com/softweb/cure/excels/LoginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="18030" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14850" windowHeight="10260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:O32"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>emails</t>
   </si>
@@ -29,6 +29,18 @@
   </si>
   <si>
     <t>bsoftwebsolutions</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>swbtop@gmail.com</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -370,7 +382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -404,13 +416,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>